<commit_message>
use the correct XLSX file with macro categorisations for 2007-13
</commit_message>
<xml_diff>
--- a/data-input/kategorizace/kategorie_0713.xlsx
+++ b/data-input/kategorizace/kategorie_0713.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/cwork/esifunguji/data-input/kategorizace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7C1CDD-59AE-EE43-AF24-83CE1D6CEEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EF2CA4-B997-0D43-BC7F-2C3482BE3FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43320" yWindow="-4100" windowWidth="25600" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="quest" sheetId="4" r:id="rId1"/>
-    <sheet name="hermin" sheetId="1" r:id="rId2"/>
-    <sheet name="prioritni_temata" sheetId="2" r:id="rId3"/>
+    <sheet name="ekonomicke_kategorie" sheetId="1" r:id="rId1"/>
+    <sheet name="prioritni_temata" sheetId="2" r:id="rId2"/>
+    <sheet name="quest_old" sheetId="4" r:id="rId3"/>
     <sheet name="kombinace" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="180">
   <si>
     <t>katekon_id</t>
   </si>
@@ -985,594 +985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9161058F-41F7-4718-9C42-057038DDFC89}">
-  <dimension ref="A1:B71"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>159</v>
-      </c>
-      <c r="B38" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>161</v>
-      </c>
-      <c r="B39" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>127</v>
-      </c>
-      <c r="B48" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>135</v>
-      </c>
-      <c r="B52" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>137</v>
-      </c>
-      <c r="B53" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>139</v>
-      </c>
-      <c r="B54" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>141</v>
-      </c>
-      <c r="B55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>145</v>
-      </c>
-      <c r="B57" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>147</v>
-      </c>
-      <c r="B58" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>149</v>
-      </c>
-      <c r="B59" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>153</v>
-      </c>
-      <c r="B61" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>163</v>
-      </c>
-      <c r="B68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>165</v>
-      </c>
-      <c r="B69" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>167</v>
-      </c>
-      <c r="B70" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>169</v>
-      </c>
-      <c r="B71" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1840,12 +1257,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1878,7 +1295,7 @@
         <v>49</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>VLOOKUP(A2,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A2,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1890,7 +1307,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>VLOOKUP(A3,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A3,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1902,7 +1319,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="5" t="str">
-        <f>VLOOKUP(A4,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A4,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1914,7 +1331,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="5" t="str">
-        <f>VLOOKUP(A5,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A5,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1926,7 +1343,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="5" t="str">
-        <f>VLOOKUP(A6,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A6,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
     </row>
@@ -1938,7 +1355,7 @@
         <v>55</v>
       </c>
       <c r="C7" s="5" t="str">
-        <f>VLOOKUP(A7,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A7,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
     </row>
@@ -1950,7 +1367,7 @@
         <v>56</v>
       </c>
       <c r="C8" s="5" t="str">
-        <f>VLOOKUP(A8,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A8,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1962,7 +1379,7 @@
         <v>57</v>
       </c>
       <c r="C9" s="5" t="str">
-        <f>VLOOKUP(A9,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A9,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
     </row>
@@ -1974,7 +1391,7 @@
         <v>58</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f>VLOOKUP(A10,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A10,quest_old!A:B,2,FALSE)</f>
         <v>RTD</v>
       </c>
     </row>
@@ -1986,11 +1403,11 @@
         <v>59</v>
       </c>
       <c r="C11" s="5" t="str">
-        <f>VLOOKUP(A11,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A11,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2001,7 +1418,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="5" t="str">
-        <f>VLOOKUP(A12,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A12,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2013,7 +1430,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="5" t="str">
-        <f>VLOOKUP(A13,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A13,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -2028,8 +1445,11 @@
         <v>62</v>
       </c>
       <c r="C14" s="5" t="str">
-        <f>VLOOKUP(A14,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A14,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2040,8 +1460,11 @@
         <v>63</v>
       </c>
       <c r="C15" s="5" t="str">
-        <f>VLOOKUP(A15,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A15,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2052,7 +1475,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="5" t="str">
-        <f>VLOOKUP(A16,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A16,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2064,7 +1487,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="5" t="str">
-        <f>VLOOKUP(A17,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A17,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2076,7 +1499,7 @@
         <v>66</v>
       </c>
       <c r="C18" s="5" t="str">
-        <f>VLOOKUP(A18,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A18,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2088,7 +1511,7 @@
         <v>67</v>
       </c>
       <c r="C19" s="5" t="str">
-        <f>VLOOKUP(A19,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A19,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2100,7 +1523,7 @@
         <v>68</v>
       </c>
       <c r="C20" s="5" t="str">
-        <f>VLOOKUP(A20,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A20,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2112,7 +1535,7 @@
         <v>69</v>
       </c>
       <c r="C21" s="5" t="str">
-        <f>VLOOKUP(A21,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A21,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2124,7 +1547,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="5" t="str">
-        <f>VLOOKUP(A22,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A22,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2136,7 +1559,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="5" t="str">
-        <f>VLOOKUP(A23,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A23,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2148,7 +1571,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="5" t="str">
-        <f>VLOOKUP(A24,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A24,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2160,7 +1583,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="5" t="str">
-        <f>VLOOKUP(A25,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A25,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2172,7 +1595,7 @@
         <v>78</v>
       </c>
       <c r="C26" s="5" t="str">
-        <f>VLOOKUP(A26,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A26,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2184,7 +1607,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="5" t="str">
-        <f>VLOOKUP(A27,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A27,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2196,7 +1619,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5" t="str">
-        <f>VLOOKUP(A28,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A28,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2208,7 +1631,7 @@
         <v>84</v>
       </c>
       <c r="C29" s="5" t="str">
-        <f>VLOOKUP(A29,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A29,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2220,7 +1643,7 @@
         <v>86</v>
       </c>
       <c r="C30" s="5" t="str">
-        <f>VLOOKUP(A30,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A30,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2232,7 +1655,7 @@
         <v>88</v>
       </c>
       <c r="C31" s="5" t="str">
-        <f>VLOOKUP(A31,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A31,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2244,7 +1667,7 @@
         <v>90</v>
       </c>
       <c r="C32" s="5" t="str">
-        <f>VLOOKUP(A32,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A32,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2256,7 +1679,7 @@
         <v>92</v>
       </c>
       <c r="C33" s="5" t="str">
-        <f>VLOOKUP(A33,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A33,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2268,7 +1691,7 @@
         <v>94</v>
       </c>
       <c r="C34" s="5" t="str">
-        <f>VLOOKUP(A34,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A34,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2280,7 +1703,7 @@
         <v>96</v>
       </c>
       <c r="C35" s="5" t="str">
-        <f>VLOOKUP(A35,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A35,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2292,7 +1715,7 @@
         <v>98</v>
       </c>
       <c r="C36" s="5" t="str">
-        <f>VLOOKUP(A36,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A36,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2304,7 +1727,7 @@
         <v>100</v>
       </c>
       <c r="C37" s="5" t="str">
-        <f>VLOOKUP(A37,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A37,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2316,7 +1739,7 @@
         <v>102</v>
       </c>
       <c r="C38" s="5" t="str">
-        <f>VLOOKUP(A38,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A38,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2328,7 +1751,7 @@
         <v>104</v>
       </c>
       <c r="C39" s="5" t="str">
-        <f>VLOOKUP(A39,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A39,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2340,7 +1763,7 @@
         <v>106</v>
       </c>
       <c r="C40" s="5" t="str">
-        <f>VLOOKUP(A40,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A40,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2352,7 +1775,7 @@
         <v>108</v>
       </c>
       <c r="C41" s="5" t="str">
-        <f>VLOOKUP(A41,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A41,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2364,7 +1787,7 @@
         <v>110</v>
       </c>
       <c r="C42" s="5" t="str">
-        <f>VLOOKUP(A42,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A42,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2376,7 +1799,7 @@
         <v>112</v>
       </c>
       <c r="C43" s="5" t="str">
-        <f>VLOOKUP(A43,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A43,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2388,7 +1811,7 @@
         <v>114</v>
       </c>
       <c r="C44" s="5" t="str">
-        <f>VLOOKUP(A44,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A44,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2400,7 +1823,7 @@
         <v>116</v>
       </c>
       <c r="C45" s="5" t="str">
-        <f>VLOOKUP(A45,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A45,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2412,7 +1835,7 @@
         <v>118</v>
       </c>
       <c r="C46" s="5" t="str">
-        <f>VLOOKUP(A46,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A46,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
     </row>
@@ -2424,11 +1847,11 @@
         <v>120</v>
       </c>
       <c r="C47" s="5" t="str">
-        <f>VLOOKUP(A47,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A47,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -2439,14 +1862,14 @@
         <v>122</v>
       </c>
       <c r="C48" s="5" t="str">
-        <f>VLOOKUP(A48,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A48,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -2454,11 +1877,14 @@
         <v>124</v>
       </c>
       <c r="C49" s="5" t="str">
-        <f>VLOOKUP(A49,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A49,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D49" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>125</v>
       </c>
@@ -2466,11 +1892,14 @@
         <v>126</v>
       </c>
       <c r="C50" s="5" t="str">
-        <f>VLOOKUP(A50,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A50,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D50" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2478,11 +1907,14 @@
         <v>128</v>
       </c>
       <c r="C51" s="5" t="str">
-        <f>VLOOKUP(A51,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A51,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="D51" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>129</v>
       </c>
@@ -2490,11 +1922,11 @@
         <v>130</v>
       </c>
       <c r="C52" s="5" t="str">
-        <f>VLOOKUP(A52,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A52,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -2502,11 +1934,11 @@
         <v>132</v>
       </c>
       <c r="C53" s="5" t="str">
-        <f>VLOOKUP(A53,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A53,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>133</v>
       </c>
@@ -2514,11 +1946,11 @@
         <v>134</v>
       </c>
       <c r="C54" s="5" t="str">
-        <f>VLOOKUP(A54,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A54,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>135</v>
       </c>
@@ -2526,11 +1958,11 @@
         <v>136</v>
       </c>
       <c r="C55" s="5" t="str">
-        <f>VLOOKUP(A55,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A55,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -2538,11 +1970,11 @@
         <v>138</v>
       </c>
       <c r="C56" s="5" t="str">
-        <f>VLOOKUP(A56,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A56,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>139</v>
       </c>
@@ -2550,11 +1982,11 @@
         <v>140</v>
       </c>
       <c r="C57" s="5" t="str">
-        <f>VLOOKUP(A57,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A57,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>141</v>
       </c>
@@ -2562,11 +1994,11 @@
         <v>142</v>
       </c>
       <c r="C58" s="5" t="str">
-        <f>VLOOKUP(A58,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A58,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -2574,11 +2006,11 @@
         <v>144</v>
       </c>
       <c r="C59" s="5" t="str">
-        <f>VLOOKUP(A59,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A59,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>145</v>
       </c>
@@ -2586,11 +2018,11 @@
         <v>146</v>
       </c>
       <c r="C60" s="5" t="str">
-        <f>VLOOKUP(A60,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A60,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>147</v>
       </c>
@@ -2598,11 +2030,11 @@
         <v>148</v>
       </c>
       <c r="C61" s="5" t="str">
-        <f>VLOOKUP(A61,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A61,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -2610,11 +2042,11 @@
         <v>150</v>
       </c>
       <c r="C62" s="5" t="str">
-        <f>VLOOKUP(A62,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A62,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>151</v>
       </c>
@@ -2622,11 +2054,11 @@
         <v>152</v>
       </c>
       <c r="C63" s="5" t="str">
-        <f>VLOOKUP(A63,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A63,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -2634,7 +2066,7 @@
         <v>154</v>
       </c>
       <c r="C64" s="5" t="str">
-        <f>VLOOKUP(A64,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A64,quest_old!A:B,2,FALSE)</f>
         <v>HC</v>
       </c>
     </row>
@@ -2646,7 +2078,7 @@
         <v>156</v>
       </c>
       <c r="C65" s="5" t="str">
-        <f>VLOOKUP(A65,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A65,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
       <c r="D65" s="5" t="s">
@@ -2661,7 +2093,7 @@
         <v>158</v>
       </c>
       <c r="C66" s="5" t="str">
-        <f>VLOOKUP(A66,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A66,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
       <c r="D66" s="5" t="s">
@@ -2676,7 +2108,7 @@
         <v>160</v>
       </c>
       <c r="C67" s="5" t="str">
-        <f>VLOOKUP(A67,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A67,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2688,7 +2120,7 @@
         <v>162</v>
       </c>
       <c r="C68" s="5" t="str">
-        <f>VLOOKUP(A68,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A68,quest_old!A:B,2,FALSE)</f>
         <v>INFR</v>
       </c>
     </row>
@@ -2700,7 +2132,7 @@
         <v>164</v>
       </c>
       <c r="C69" s="5" t="str">
-        <f>VLOOKUP(A69,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A69,quest_old!A:B,2,FALSE)</f>
         <v>TA</v>
       </c>
     </row>
@@ -2712,7 +2144,7 @@
         <v>166</v>
       </c>
       <c r="C70" s="5" t="str">
-        <f>VLOOKUP(A70,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A70,quest_old!A:B,2,FALSE)</f>
         <v>TA</v>
       </c>
     </row>
@@ -2724,7 +2156,7 @@
         <v>168</v>
       </c>
       <c r="C71" s="5" t="str">
-        <f>VLOOKUP(A71,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A71,quest_old!A:B,2,FALSE)</f>
         <v>TA</v>
       </c>
     </row>
@@ -2736,8 +2168,591 @@
         <v>170</v>
       </c>
       <c r="C72" s="5" t="str">
-        <f>VLOOKUP(A72,quest!A:B,2,FALSE)</f>
+        <f>VLOOKUP(A72,quest_old!A:B,2,FALSE)</f>
         <v>TA</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9161058F-41F7-4718-9C42-057038DDFC89}">
+  <dimension ref="A1:B71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolve 2007-13 HERMIN categories and export data
</commit_message>
<xml_diff>
--- a/data-input/kategorizace/kategorie_0713.xlsx
+++ b/data-input/kategorizace/kategorie_0713.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11202"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/cwork/esifunguji/data-input/kategorizace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EF2CA4-B997-0D43-BC7F-2C3482BE3FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BFEA7E-335E-0541-83E5-09A7DB0699FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ekonomicke_kategorie" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="180">
   <si>
     <t>katekon_id</t>
   </si>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1837,6 +1837,9 @@
       <c r="C46" s="5" t="str">
         <f>VLOOKUP(A46,quest_old!A:B,2,FALSE)</f>
         <v>AIS</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>